<commit_message>
apresentação pré finalizada e melhorias na documentação
</commit_message>
<xml_diff>
--- a/TCC/PTCC/Outros/Rascunho_proj/Cronograma.xlsx
+++ b/TCC/PTCC/Outros/Rascunho_proj/Cronograma.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Etec\TCC\PTCC\Outros\Rascunho_proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erics\Documents\GitHub\tccETEC\Etec\TCC\PTCC\Outros\Rascunho_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FC137C-4724-4FE4-956B-D61DB9B63B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
+    <workbookView xWindow="-19320" yWindow="2595" windowWidth="19440" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Inicio</t>
   </si>
@@ -127,14 +128,35 @@
     <t>CRUD Agendamento Salão</t>
   </si>
   <si>
-    <t>CRUD Vaga Proprietarios</t>
+    <t>CRUD Minha Vaga</t>
+  </si>
+  <si>
+    <t>Documentação dos sites</t>
+  </si>
+  <si>
+    <t>CRUD Proprietarios</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Revisão da documentação</t>
+  </si>
+  <si>
+    <t>Eric e João</t>
+  </si>
+  <si>
+    <t>CRUD Meu Cadastro</t>
+  </si>
+  <si>
+    <t>Tela inicial da Shannon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,8 +179,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,8 +200,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -279,12 +314,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -292,17 +353,10 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,6 +383,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -359,13 +431,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>158750</xdr:colOff>
+      <xdr:colOff>172085</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1072732</xdr:rowOff>
+      <xdr:rowOff>1074637</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -659,55 +737,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G28" sqref="B2:G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="3" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="3" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="1" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -727,377 +805,485 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
         <v>44775</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4" t="str">
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+      <c r="G6" s="20" t="str">
         <f>IF(F6&lt;=30%,"Primicias",IF(F6&lt;5=50%,"Em Desenvolvimento",IF(F6&lt;=99%,"No finalmente","Concluido")))</f>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="10">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
         <v>44775</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4" t="str">
+      <c r="F7" s="21">
+        <v>1</v>
+      </c>
+      <c r="G7" s="20" t="str">
         <f t="shared" ref="G7:G18" si="0">IF(F7&lt;=30%,"Primicias",IF(F7&lt;5=50%,"Em Desenvolvimento",IF(F7&lt;=99%,"No finalmente","Concluido")))</f>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
         <v>44775</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4" t="str">
+      <c r="F8" s="21">
+        <v>1</v>
+      </c>
+      <c r="G8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="5">
         <v>44786</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>44789</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4" t="str">
+      <c r="F9" s="21">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="10">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
         <v>44796</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="5">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4" t="str">
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+      <c r="G10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="10">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
         <v>44817</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4" t="str">
+      <c r="F11" s="21">
+        <v>1</v>
+      </c>
+      <c r="G11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10">
+    <row r="12" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="16">
         <v>44820</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8" t="str">
+      <c r="F12" s="21">
+        <v>1</v>
+      </c>
+      <c r="G12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="10">
+    <row r="13" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="7">
         <v>44820</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="5">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4" t="str">
+      <c r="F13" s="21">
+        <v>1</v>
+      </c>
+      <c r="G13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="5">
         <v>44822</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="5">
-        <v>0.85</v>
-      </c>
-      <c r="G14" s="4" t="str">
+      <c r="F14" s="21">
+        <v>1</v>
+      </c>
+      <c r="G14" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>No finalmente</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+        <v>Concluido</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="5">
         <v>44830</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>44838</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="5">
-        <v>1</v>
-      </c>
-      <c r="G15" s="4" t="str">
+      <c r="F15" s="21">
+        <v>1</v>
+      </c>
+      <c r="G15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
         <v>44850</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>44850</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="5">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4" t="str">
+      <c r="F16" s="21">
+        <v>1</v>
+      </c>
+      <c r="G16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
         <v>44887</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>44887</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="5">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4" t="str">
+      <c r="F17" s="21">
+        <v>1</v>
+      </c>
+      <c r="G17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
         <v>44894</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>44894</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="5">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4" t="str">
+      <c r="F18" s="21">
+        <v>1</v>
+      </c>
+      <c r="G18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
         <v>44894</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>44894</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="4" t="str">
-        <f t="shared" ref="G19:G22" si="1">IF(F19&lt;=30%,"Primicias",IF(F19&lt;5=50%,"Em Desenvolvimento",IF(F19&lt;=99%,"No finalmente","Concluido")))</f>
-        <v>Concluido</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
-        <v>44897</v>
-      </c>
-      <c r="C20" s="6">
-        <v>44936</v>
+      <c r="F19" s="21">
+        <v>1</v>
+      </c>
+      <c r="G19" s="20" t="str">
+        <f t="shared" ref="G19:G23" si="1">IF(F19&lt;=30%,"Primicias",IF(F19&lt;5=50%,"Em Desenvolvimento",IF(F19&lt;=99%,"No finalmente","Concluido")))</f>
+        <v>Concluido</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>45020</v>
+      </c>
+      <c r="C20" s="5">
+        <v>45034</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="21">
+        <v>1</v>
+      </c>
+      <c r="G20" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Concluido</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>44977</v>
+      </c>
+      <c r="C21" s="5">
+        <v>45041</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="20" t="str">
+        <f>IF(F21&lt;=30%,"Primicias",IF(F21&lt;5=50%,"Em Desenvolvimento",IF(F21&lt;=99%,"No finalmente","Concluido")))</f>
+        <v>Concluido</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>44992</v>
+      </c>
+      <c r="C22" s="5">
+        <v>45048</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E22" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="5">
-        <v>1</v>
-      </c>
-      <c r="G20" s="4" t="str">
+      <c r="F22" s="21">
+        <v>1</v>
+      </c>
+      <c r="G22" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="6">
-        <v>44946</v>
-      </c>
-      <c r="C21" s="6">
-        <v>44957</v>
-      </c>
-      <c r="D21" s="4" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="5">
+        <v>45006</v>
+      </c>
+      <c r="C23" s="5">
+        <v>45055</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E23" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="5">
-        <v>1</v>
-      </c>
-      <c r="G21" s="4" t="str">
+      <c r="F23" s="21">
+        <v>1</v>
+      </c>
+      <c r="G23" s="20" t="str">
         <f t="shared" si="1"/>
         <v>Concluido</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
-        <v>44977</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>45019</v>
+      </c>
+      <c r="C24" s="5">
+        <v>45069</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="G22" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>No finalmente</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
-        <v>45018</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4" t="s">
+      <c r="F24" s="21">
+        <v>1</v>
+      </c>
+      <c r="G24" s="20" t="str">
+        <f t="shared" ref="G24" si="2">IF(F24&lt;=30%,"Primicias",IF(F24&lt;5=50%,"Em Desenvolvimento",IF(F24&lt;=99%,"No finalmente","Concluido")))</f>
+        <v>Concluido</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="5">
+        <v>45041</v>
+      </c>
+      <c r="C25" s="5">
+        <v>45083</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="G23" s="4" t="str">
-        <f t="shared" ref="G23" si="2">IF(F23&lt;=30%,"Primicias",IF(F23&lt;5=50%,"Em Desenvolvimento",IF(F23&lt;=99%,"No finalmente","Concluido")))</f>
-        <v>No finalmente</v>
+      <c r="F25" s="21">
+        <v>1</v>
+      </c>
+      <c r="G25" s="20" t="str">
+        <f t="shared" ref="G25:G26" si="3">IF(F25&lt;=30%,"Primicias",IF(F25&lt;5=50%,"Em Desenvolvimento",IF(F25&lt;=99%,"No finalmente","Concluido")))</f>
+        <v>Concluido</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="5">
+        <v>45020</v>
+      </c>
+      <c r="C26" s="5">
+        <v>45083</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="21">
+        <v>1</v>
+      </c>
+      <c r="G26" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>Concluido</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="5">
+        <v>44782</v>
+      </c>
+      <c r="C27" s="5">
+        <v>45083</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="21">
+        <v>1</v>
+      </c>
+      <c r="G27" s="20" t="str">
+        <f t="shared" ref="G27:G28" si="4">IF(F27&lt;=30%,"Primicias",IF(F27&lt;5=50%,"Em Desenvolvimento",IF(F27&lt;=99%,"No finalmente","Concluido")))</f>
+        <v>Concluido</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="18">
+        <v>45084</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="21">
+        <v>1</v>
+      </c>
+      <c r="G28" s="20" t="str">
+        <f t="shared" si="4"/>
+        <v>Concluido</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
+  <mergeCells count="12">
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>